<commit_message>
fixed linking issue. Pages now opening from the links
</commit_message>
<xml_diff>
--- a/Error List.xlsx
+++ b/Error List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Error list</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Project-properties -&gt; Java Compiler-&gt;JDK compliance-&gt;Compiler Compliance Level = 1.5</t>
+  </si>
+  <si>
+    <t>eclipse-error-the-import-xxx-cannot-be-resolved</t>
+  </si>
+  <si>
+    <t>Go to project in the task view and click on Clean..</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +402,14 @@
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jstl code added- hibernate not working yet
</commit_message>
<xml_diff>
--- a/Error List.xlsx
+++ b/Error List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Error list</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Go to project in the task view and click on Clean..</t>
+  </si>
+  <si>
+    <t>No mapping found for HTTP request with URI [/muziqhub/] in DispatcherServlet with name 'dispatcher'</t>
+  </si>
+  <si>
+    <t>Project properties-&gt; Facets-&gt;Runtime-&gt; add tomcat</t>
+  </si>
+  <si>
+    <t>Attribute item invalid for tag forEach according to TLD</t>
+  </si>
+  <si>
+    <t>Add jstl dependencies in pom.xml</t>
   </si>
 </sst>
 </file>
@@ -372,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,6 +422,22 @@
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tables generated through hibernate in H2
</commit_message>
<xml_diff>
--- a/Error List.xlsx
+++ b/Error List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Error list</t>
   </si>
@@ -46,6 +46,16 @@
   </si>
   <si>
     <t>Add jstl dependencies in pom.xml</t>
+  </si>
+  <si>
+    <t>Cannot find class [org.springframework.jdbc.datasource.DriverManagerDataSource] for bean with name 'dataSource'</t>
+  </si>
+  <si>
+    <t>add &lt;dependency&gt;
+    &lt;groupId&gt;org.springframework&lt;/groupId&gt;
+    &lt;artifactId&gt;spring-jdbc&lt;/artifactId&gt;
+    &lt;version&gt;3.0.3.RELEASE&lt;/version&gt;
+&lt;/dependency&gt;  in pom</t>
   </si>
 </sst>
 </file>
@@ -81,8 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +451,14 @@
       </c>
       <c r="B6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>